<commit_message>
update get finish project
</commit_message>
<xml_diff>
--- a/services/retrain/finish_project.xlsx
+++ b/services/retrain/finish_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duy\Github\doccano-plugin\services\retrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0B30E5-F681-4573-A001-71A949D5170F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4646EBB6-7843-4926-A6B6-89D3C25B2834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,13 +53,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,22 +87,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,30 +455,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D9" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>